<commit_message>
reading and storing bytes
</commit_message>
<xml_diff>
--- a/efr3214fg_opamp_adc_readings.xlsx
+++ b/efr3214fg_opamp_adc_readings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Co-op Shaheeer R\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C839FC2F-F72C-4A8D-B27D-760758B15389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC15634-5C24-4AEB-BD74-B34AD8EA61FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22020" yWindow="0" windowWidth="16320" windowHeight="17085" activeTab="4" xr2:uid="{123C8E70-5E88-486D-BEC0-EE819F103977}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="10920" firstSheet="1" activeTab="3" xr2:uid="{123C8E70-5E88-486D-BEC0-EE819F103977}"/>
   </bookViews>
   <sheets>
     <sheet name="2 Cascading Inverting Opamps" sheetId="1" r:id="rId1"/>
@@ -6799,8 +6799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA2608C-9641-4248-BCF8-810721F8EA22}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6841,7 +6841,7 @@
         <v>-7.62939453125E-2</v>
       </c>
       <c r="F2" t="e">
-        <f>E2/B2*100</f>
+        <f>ABS(E2-B2)/B2*100</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -6865,13 +6865,13 @@
         <v>5.46875E-2</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F52" si="2">E3/B3*100</f>
-        <v>0.12428977272727272</v>
+        <f>ABS(E3-B3)/B3*100</f>
+        <v>99.875710227272734</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A50" si="3">A3+50</f>
+        <f t="shared" ref="A4:A50" si="2">A3+50</f>
         <v>100</v>
       </c>
       <c r="B4">
@@ -6889,13 +6889,13 @@
         <v>-0.24481201171875</v>
       </c>
       <c r="F4">
-        <f t="shared" si="2"/>
-        <v>-0.25501251220703125</v>
+        <f t="shared" ref="F4:F52" si="3">ABS(E4-B4)/B4*100</f>
+        <v>100.25501251220703</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="B5">
@@ -6913,13 +6913,13 @@
         <v>-1.078369140625</v>
       </c>
       <c r="F5">
-        <f t="shared" si="2"/>
-        <v>-0.72862779771959452</v>
+        <f t="shared" si="3"/>
+        <v>100.72862779771961</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>200</v>
       </c>
       <c r="B6">
@@ -6937,13 +6937,13 @@
         <v>-2.67486572265625</v>
       </c>
       <c r="F6">
-        <f t="shared" si="2"/>
-        <v>-1.337432861328125</v>
+        <f t="shared" si="3"/>
+        <v>101.33743286132813</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>250</v>
       </c>
       <c r="B7">
@@ -6961,13 +6961,13 @@
         <v>-1.364013671875</v>
       </c>
       <c r="F7">
-        <f t="shared" si="2"/>
-        <v>-0.53913583868577075</v>
+        <f t="shared" si="3"/>
+        <v>100.53913583868577</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>300</v>
       </c>
       <c r="B8">
@@ -6985,13 +6985,13 @@
         <v>-2.647216796875</v>
       </c>
       <c r="F8">
-        <f t="shared" si="2"/>
-        <v>-0.90658109482020555</v>
+        <f t="shared" si="3"/>
+        <v>100.9065810948202</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>350</v>
       </c>
       <c r="B9">
@@ -7009,13 +7009,13 @@
         <v>-1.03936767578125</v>
       </c>
       <c r="F9">
-        <f t="shared" si="2"/>
-        <v>-0.30214176621547967</v>
+        <f t="shared" si="3"/>
+        <v>100.30214176621548</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>400</v>
       </c>
       <c r="B10">
@@ -7033,13 +7033,13 @@
         <v>0.23333740234375</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
-        <v>5.8775164318324934E-2</v>
+        <f t="shared" si="3"/>
+        <v>99.94122483568168</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>450</v>
       </c>
       <c r="B11">
@@ -7057,13 +7057,13 @@
         <v>-0.8291015625</v>
       </c>
       <c r="F11">
-        <f t="shared" si="2"/>
-        <v>-0.18465513641425388</v>
+        <f t="shared" si="3"/>
+        <v>100.18465513641426</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>500</v>
       </c>
       <c r="B12">
@@ -7081,13 +7081,13 @@
         <v>-9.04541015625E-2</v>
       </c>
       <c r="F12">
-        <f t="shared" si="2"/>
-        <v>-1.8018745331175298E-2</v>
+        <f t="shared" si="3"/>
+        <v>100.01801874533118</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>550</v>
       </c>
       <c r="B13">
@@ -7105,13 +7105,13 @@
         <v>-0.50439453125</v>
       </c>
       <c r="F13">
-        <f t="shared" si="2"/>
-        <v>-9.1045944268953072E-2</v>
+        <f t="shared" si="3"/>
+        <v>100.09104594426897</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>600</v>
       </c>
       <c r="B14">
@@ -7129,13 +7129,13 @@
         <v>-1.024658203125</v>
       </c>
       <c r="F14">
-        <f t="shared" si="2"/>
-        <v>-0.17279227708684655</v>
+        <f t="shared" si="3"/>
+        <v>100.17279227708684</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>650</v>
       </c>
       <c r="B15">
@@ -7153,13 +7153,13 @@
         <v>-1.24786376953125</v>
       </c>
       <c r="F15">
-        <f t="shared" si="2"/>
-        <v>-0.19346725109011628</v>
+        <f t="shared" si="3"/>
+        <v>100.19346725109011</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>700</v>
       </c>
       <c r="B16">
@@ -7177,13 +7177,13 @@
         <v>-1.19586181640625</v>
       </c>
       <c r="F16">
-        <f t="shared" si="2"/>
-        <v>-0.1713269077945917</v>
+        <f t="shared" si="3"/>
+        <v>100.17132690779459</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>750</v>
       </c>
       <c r="B17">
@@ -7201,13 +7201,13 @@
         <v>-0.732421875</v>
       </c>
       <c r="F17">
-        <f t="shared" si="2"/>
-        <v>-9.765625E-2</v>
+        <f t="shared" si="3"/>
+        <v>100.09765625</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>800</v>
       </c>
       <c r="B18">
@@ -7225,13 +7225,13 @@
         <v>-1.26080322265625</v>
       </c>
       <c r="F18">
-        <f t="shared" si="2"/>
-        <v>-0.15720738437110349</v>
+        <f t="shared" si="3"/>
+        <v>100.15720738437111</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>850</v>
       </c>
       <c r="B19">
@@ -7249,8 +7249,8 @@
         <v>-2.01806640625</v>
       </c>
       <c r="F19">
-        <f t="shared" si="2"/>
-        <v>-0.23630754171545665</v>
+        <f t="shared" si="3"/>
+        <v>100.23630754171546</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -7273,13 +7273,13 @@
         <v>-2.4620361328125</v>
       </c>
       <c r="F20">
-        <f t="shared" si="2"/>
-        <v>-0.2757039342455207</v>
+        <f t="shared" si="3"/>
+        <v>100.27570393424551</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>950</v>
       </c>
       <c r="B21">
@@ -7297,13 +7297,13 @@
         <v>-2.14300537109375</v>
       </c>
       <c r="F21">
-        <f t="shared" si="2"/>
-        <v>-0.2265333373249207</v>
+        <f t="shared" si="3"/>
+        <v>100.22653333732492</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="B22">
@@ -7321,13 +7321,13 @@
         <v>-2.63323974609375</v>
       </c>
       <c r="F22">
-        <f t="shared" si="2"/>
-        <v>-0.26385167796530562</v>
+        <f t="shared" si="3"/>
+        <v>100.26385167796531</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1050</v>
       </c>
       <c r="B23">
@@ -7345,13 +7345,13 @@
         <v>-2.398681640625</v>
       </c>
       <c r="F23">
-        <f t="shared" si="2"/>
-        <v>-0.2284458705357143</v>
+        <f t="shared" si="3"/>
+        <v>100.22844587053572</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1100</v>
       </c>
       <c r="B24">
@@ -7369,13 +7369,13 @@
         <v>-1.85076904296875</v>
       </c>
       <c r="F24">
-        <f t="shared" si="2"/>
-        <v>-0.16779411087658658</v>
+        <f t="shared" si="3"/>
+        <v>100.1677941108766</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1150</v>
       </c>
       <c r="B25">
@@ -7393,13 +7393,13 @@
         <v>-1.8450927734375</v>
       </c>
       <c r="F25">
-        <f t="shared" si="2"/>
-        <v>-0.15974829207251082</v>
+        <f t="shared" si="3"/>
+        <v>100.15974829207251</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1200</v>
       </c>
       <c r="B26">
@@ -7417,13 +7417,13 @@
         <v>-0.831298828125</v>
       </c>
       <c r="F26">
-        <f t="shared" si="2"/>
-        <v>-6.9564755491631797E-2</v>
+        <f t="shared" si="3"/>
+        <v>100.06956475549163</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1250</v>
       </c>
       <c r="B27">
@@ -7441,13 +7441,13 @@
         <v>-3.237060546875</v>
       </c>
       <c r="F27">
-        <f t="shared" si="2"/>
-        <v>-0.2597961915630016</v>
+        <f t="shared" si="3"/>
+        <v>100.259796191563</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1300</v>
       </c>
       <c r="B28">
@@ -7465,13 +7465,13 @@
         <v>-2.99432373046875</v>
       </c>
       <c r="F28">
-        <f t="shared" si="2"/>
-        <v>-0.2305099099668014</v>
+        <f t="shared" si="3"/>
+        <v>100.2305099099668</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1350</v>
       </c>
       <c r="B29">
@@ -7489,13 +7489,13 @@
         <v>-2.17938232421875</v>
       </c>
       <c r="F29">
-        <f t="shared" si="2"/>
-        <v>-0.16119691747180104</v>
+        <f t="shared" si="3"/>
+        <v>100.16119691747181</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1400</v>
       </c>
       <c r="B30">
@@ -7513,13 +7513,13 @@
         <v>-4.27996826171875</v>
       </c>
       <c r="F30">
-        <f t="shared" si="2"/>
-        <v>-0.30505832228929081</v>
+        <f t="shared" si="3"/>
+        <v>100.30505832228928</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1450</v>
       </c>
       <c r="B31">
@@ -7537,8 +7537,8 @@
         <v>-4.3043212890625</v>
       </c>
       <c r="F31">
-        <f t="shared" si="2"/>
-        <v>-0.29849662198769067</v>
+        <f t="shared" si="3"/>
+        <v>100.29849662198768</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -7561,13 +7561,13 @@
         <v>-4.7100830078125</v>
       </c>
       <c r="F32">
-        <f t="shared" si="2"/>
-        <v>-0.31505571958612039</v>
+        <f t="shared" si="3"/>
+        <v>100.31505571958613</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1550</v>
       </c>
       <c r="B33">
@@ -7585,13 +7585,13 @@
         <v>-3.02593994140625</v>
       </c>
       <c r="F33">
-        <f t="shared" si="2"/>
-        <v>-0.1956005133423562</v>
+        <f t="shared" si="3"/>
+        <v>100.19560051334236</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1600</v>
       </c>
       <c r="B34">
@@ -7609,13 +7609,13 @@
         <v>-3.13470458984375</v>
       </c>
       <c r="F34">
-        <f t="shared" si="2"/>
-        <v>-0.19604156284201063</v>
+        <f t="shared" si="3"/>
+        <v>100.19604156284201</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1650</v>
       </c>
       <c r="B35">
@@ -7633,13 +7633,13 @@
         <v>-3.1044921875</v>
       </c>
       <c r="F35">
-        <f t="shared" si="2"/>
-        <v>-0.1876960210096735</v>
+        <f t="shared" si="3"/>
+        <v>100.18769602100967</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1700</v>
       </c>
       <c r="B36">
@@ -7657,13 +7657,13 @@
         <v>-3.8236083984375</v>
       </c>
       <c r="F36">
-        <f t="shared" si="2"/>
-        <v>-0.22412710424604335</v>
+        <f t="shared" si="3"/>
+        <v>100.22412710424604</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1750</v>
       </c>
       <c r="B37">
@@ -7681,13 +7681,13 @@
         <v>-3.96240234375</v>
       </c>
       <c r="F37">
-        <f t="shared" si="2"/>
-        <v>-0.22707176755014327</v>
+        <f t="shared" si="3"/>
+        <v>100.22707176755014</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1800</v>
       </c>
       <c r="B38">
@@ -7705,13 +7705,13 @@
         <v>-4.18560791015625</v>
       </c>
       <c r="F38">
-        <f t="shared" si="2"/>
-        <v>-0.23292197607992488</v>
+        <f t="shared" si="3"/>
+        <v>100.23292197607991</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1850</v>
       </c>
       <c r="B39">
@@ -7729,13 +7729,13 @@
         <v>-4.36248779296875</v>
       </c>
       <c r="F39">
-        <f t="shared" si="2"/>
-        <v>-0.2358101509712838</v>
+        <f t="shared" si="3"/>
+        <v>100.23581015097129</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1900</v>
       </c>
       <c r="B40">
@@ -7753,13 +7753,13 @@
         <v>-5.2723388671875</v>
       </c>
       <c r="F40">
-        <f t="shared" si="2"/>
-        <v>-0.27719973013604099</v>
+        <f t="shared" si="3"/>
+        <v>100.27719973013605</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1950</v>
       </c>
       <c r="B41">
@@ -7777,13 +7777,13 @@
         <v>-4.04595947265625</v>
       </c>
       <c r="F41">
-        <f t="shared" si="2"/>
-        <v>-0.20706036195784289</v>
+        <f t="shared" si="3"/>
+        <v>100.20706036195783</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="B42">
@@ -7801,8 +7801,8 @@
         <v>-3.498046875</v>
       </c>
       <c r="F42">
-        <f t="shared" si="2"/>
-        <v>-0.1742923206278027</v>
+        <f t="shared" si="3"/>
+        <v>100.1742923206278</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -7825,13 +7825,13 @@
         <v>-3.4842529296875</v>
       </c>
       <c r="F43">
-        <f t="shared" si="2"/>
-        <v>-0.17029584211571358</v>
+        <f t="shared" si="3"/>
+        <v>100.17029584211572</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2100</v>
       </c>
       <c r="B44">
@@ -7849,13 +7849,13 @@
         <v>-3.6693115234375</v>
       </c>
       <c r="F44">
-        <f t="shared" si="2"/>
-        <v>-0.17489568748510487</v>
+        <f t="shared" si="3"/>
+        <v>100.1748956874851</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2150</v>
       </c>
       <c r="B45">
@@ -7873,13 +7873,13 @@
         <v>-5.34210205078125</v>
       </c>
       <c r="F45">
-        <f t="shared" si="2"/>
-        <v>-0.2484698628270349</v>
+        <f t="shared" si="3"/>
+        <v>100.24846986282702</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2200</v>
       </c>
       <c r="B46">
@@ -7897,13 +7897,13 @@
         <v>-4.60345458984375</v>
       </c>
       <c r="F46">
-        <f t="shared" si="2"/>
-        <v>-0.20896298637511349</v>
+        <f t="shared" si="3"/>
+        <v>100.20896298637511</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2250</v>
       </c>
       <c r="B47">
@@ -7921,13 +7921,13 @@
         <v>-3.41522216796875</v>
       </c>
       <c r="F47">
-        <f t="shared" si="2"/>
-        <v>-0.15145109392322614</v>
+        <f t="shared" si="3"/>
+        <v>100.15145109392323</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2300</v>
       </c>
       <c r="B48">
@@ -7945,13 +7945,13 @@
         <v>-5.20245361328125</v>
       </c>
       <c r="F48">
-        <f t="shared" si="2"/>
-        <v>-0.22550730876815128</v>
+        <f t="shared" si="3"/>
+        <v>100.22550730876816</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2350</v>
       </c>
       <c r="B49">
@@ -7969,13 +7969,13 @@
         <v>-5.35504150390625</v>
       </c>
       <c r="F49">
-        <f t="shared" si="2"/>
-        <v>-0.2321214349330841</v>
+        <f t="shared" si="3"/>
+        <v>100.23212143493308</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2400</v>
       </c>
       <c r="B50">
@@ -7993,8 +7993,8 @@
         <v>-4.25927734375</v>
       </c>
       <c r="F50">
-        <f t="shared" si="2"/>
-        <v>-0.17754386593372237</v>
+        <f t="shared" si="3"/>
+        <v>100.17754386593371</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -8017,8 +8017,8 @@
         <v>-4.78765869140625</v>
       </c>
       <c r="F51">
-        <f t="shared" si="2"/>
-        <v>-0.19533491193007954</v>
+        <f t="shared" si="3"/>
+        <v>100.19533491193009</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -8041,8 +8041,8 @@
         <v>4.6103515625</v>
       </c>
       <c r="F52">
-        <f t="shared" si="2"/>
-        <v>0.18411947134584666</v>
+        <f t="shared" si="3"/>
+        <v>99.815880528654162</v>
       </c>
     </row>
   </sheetData>
@@ -8054,7 +8054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6854D688-D383-4E07-8019-FC9E244BF918}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>

</xml_diff>